<commit_message>
Actualización de archivos JSON y scripts 01 de septiembre
</commit_message>
<xml_diff>
--- a/Segumiento_Tuya.xlsx
+++ b/Segumiento_Tuya.xlsx
@@ -1310,6 +1310,9 @@
     <xf borderId="5" fillId="3" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf borderId="5" fillId="3" fontId="11" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
     <xf borderId="5" fillId="3" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1318,9 +1321,6 @@
     </xf>
     <xf borderId="5" fillId="3" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="3" fontId="11" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="5" fillId="4" fontId="11" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" vertical="center"/>
@@ -1917,7 +1917,7 @@
       <c r="L2" s="22"/>
       <c r="M2" s="23">
         <f>IF(ISBLANK(L2), NETWORKDAYS(J2, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J2, L2, Hoja2!$A$1:$A$18))</f>
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="N2" s="24"/>
       <c r="O2" s="25"/>
@@ -1979,7 +1979,7 @@
       <c r="L3" s="37"/>
       <c r="M3" s="38">
         <f>IF(ISBLANK(L3), NETWORKDAYS(J3, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J3, L3, Hoja2!$A$1:$A$18))</f>
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="N3" s="39"/>
       <c r="O3" s="40"/>
@@ -2041,7 +2041,7 @@
       <c r="L4" s="22"/>
       <c r="M4" s="23">
         <f>IF(ISBLANK(L4), NETWORKDAYS(J4, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J4, L4, Hoja2!$A$1:$A$18))</f>
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="N4" s="22"/>
       <c r="O4" s="25"/>
@@ -2103,7 +2103,7 @@
       <c r="L5" s="36"/>
       <c r="M5" s="38">
         <f>IF(ISBLANK(L5), NETWORKDAYS(J5, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J5, L5, Hoja2!$A$1:$A$18))</f>
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="N5" s="39"/>
       <c r="O5" s="40"/>
@@ -2165,7 +2165,7 @@
       <c r="L6" s="22"/>
       <c r="M6" s="23">
         <f>IF(ISBLANK(L6), NETWORKDAYS(J6, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J6, L6, Hoja2!$A$1:$A$18))</f>
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="N6" s="24"/>
       <c r="O6" s="25"/>
@@ -2227,7 +2227,7 @@
       <c r="L7" s="45"/>
       <c r="M7" s="38">
         <f>IF(ISBLANK(L7), NETWORKDAYS(J7, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J7, L7, Hoja2!$A$1:$A$18))</f>
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="N7" s="46"/>
       <c r="O7" s="47"/>
@@ -2289,7 +2289,7 @@
       <c r="L8" s="22"/>
       <c r="M8" s="23">
         <f>IF(ISBLANK(L8), NETWORKDAYS(J8, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J8, L8, Hoja2!$A$1:$A$18))</f>
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="N8" s="22"/>
       <c r="O8" s="50"/>
@@ -2351,7 +2351,7 @@
       <c r="L9" s="36"/>
       <c r="M9" s="38">
         <f>IF(ISBLANK(L9), NETWORKDAYS(J9, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J9, L9, Hoja2!$A$1:$A$18))</f>
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="N9" s="46"/>
       <c r="O9" s="47"/>
@@ -2413,7 +2413,7 @@
       <c r="L10" s="22"/>
       <c r="M10" s="23">
         <f>IF(ISBLANK(L10), NETWORKDAYS(J16, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J16, L10, Hoja2!$A$1:$A$18))</f>
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="N10" s="22"/>
       <c r="O10" s="50"/>
@@ -2768,7 +2768,7 @@
       <c r="L16" s="22"/>
       <c r="M16" s="23">
         <f>IF(ISBLANK(L16), NETWORKDAYS(J17, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J17, L16, Hoja2!$A$1:$A$18))</f>
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="N16" s="22"/>
       <c r="O16" s="50"/>
@@ -2828,7 +2828,7 @@
       <c r="L17" s="37"/>
       <c r="M17" s="38">
         <f>IF(ISBLANK(L17), NETWORKDAYS(J18, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J18, L17, Hoja2!$A$1:$A$18))</f>
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="N17" s="37"/>
       <c r="O17" s="47"/>
@@ -2888,7 +2888,7 @@
       <c r="L18" s="22"/>
       <c r="M18" s="23">
         <f>IF(ISBLANK(L18), NETWORKDAYS(J19, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J19, L18, Hoja2!$A$1:$A$18))</f>
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="N18" s="22"/>
       <c r="O18" s="50"/>
@@ -2948,7 +2948,7 @@
       <c r="L19" s="37"/>
       <c r="M19" s="38">
         <f>IF(ISBLANK(L19), NETWORKDAYS(J20, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J20, L19, Hoja2!$A$1:$A$18))</f>
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="N19" s="37"/>
       <c r="O19" s="47"/>
@@ -3008,7 +3008,7 @@
       <c r="L20" s="87"/>
       <c r="M20" s="23">
         <f>IF(ISBLANK(L20), NETWORKDAYS(J21, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J21, L20, Hoja2!$A$1:$A$18))</f>
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N20" s="90"/>
       <c r="O20" s="50"/>
@@ -3253,11 +3253,11 @@
       </c>
       <c r="H24" s="68"/>
       <c r="I24" s="90"/>
-      <c r="J24" s="77">
+      <c r="J24" s="69">
         <v>45860.0</v>
       </c>
       <c r="K24" s="87"/>
-      <c r="L24" s="87">
+      <c r="L24" s="99">
         <v>45860.0</v>
       </c>
       <c r="M24" s="23">
@@ -3266,7 +3266,7 @@
       </c>
       <c r="N24" s="90"/>
       <c r="O24" s="50"/>
-      <c r="P24" s="99"/>
+      <c r="P24" s="100"/>
       <c r="Q24" s="27" t="b">
         <v>1</v>
       </c>
@@ -3303,7 +3303,7 @@
       <c r="C25" s="94" t="s">
         <v>97</v>
       </c>
-      <c r="D25" s="100" t="s">
+      <c r="D25" s="101" t="s">
         <v>98</v>
       </c>
       <c r="E25" s="95"/>
@@ -3363,7 +3363,7 @@
       <c r="C26" s="97" t="s">
         <v>100</v>
       </c>
-      <c r="D26" s="101" t="s">
+      <c r="D26" s="102" t="s">
         <v>101</v>
       </c>
       <c r="E26" s="98"/>
@@ -3379,7 +3379,7 @@
         <v>45856.0</v>
       </c>
       <c r="K26" s="87"/>
-      <c r="L26" s="102">
+      <c r="L26" s="99">
         <v>45861.0</v>
       </c>
       <c r="M26" s="23">
@@ -3507,7 +3507,7 @@
         <v>45874.0</v>
       </c>
       <c r="K28" s="87"/>
-      <c r="L28" s="102">
+      <c r="L28" s="99">
         <v>45875.0</v>
       </c>
       <c r="M28" s="23">
@@ -3516,7 +3516,7 @@
       </c>
       <c r="N28" s="90"/>
       <c r="O28" s="50"/>
-      <c r="P28" s="99"/>
+      <c r="P28" s="100"/>
       <c r="Q28" s="27" t="b">
         <v>1</v>
       </c>
@@ -3553,7 +3553,7 @@
       <c r="C29" s="94" t="s">
         <v>111</v>
       </c>
-      <c r="D29" s="100" t="s">
+      <c r="D29" s="101" t="s">
         <v>112</v>
       </c>
       <c r="E29" s="108"/>
@@ -3617,7 +3617,7 @@
       <c r="C30" s="97" t="s">
         <v>115</v>
       </c>
-      <c r="D30" s="101" t="s">
+      <c r="D30" s="102" t="s">
         <v>116</v>
       </c>
       <c r="E30" s="105"/>
@@ -3633,7 +3633,7 @@
         <v>45884.0</v>
       </c>
       <c r="K30" s="87"/>
-      <c r="L30" s="102">
+      <c r="L30" s="99">
         <v>45889.0</v>
       </c>
       <c r="M30" s="23">
@@ -3681,7 +3681,7 @@
       <c r="C31" s="111" t="s">
         <v>119</v>
       </c>
-      <c r="D31" s="100" t="s">
+      <c r="D31" s="101" t="s">
         <v>120</v>
       </c>
       <c r="E31" s="108"/>
@@ -3748,11 +3748,11 @@
       <c r="L32" s="87"/>
       <c r="M32" s="23">
         <f>IF(ISBLANK(L32), NETWORKDAYS(J33, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J33, L32, Hoja2!$A$1:$A$18))</f>
-        <v>32768</v>
+        <v>32770</v>
       </c>
       <c r="N32" s="90"/>
       <c r="O32" s="50"/>
-      <c r="P32" s="99"/>
+      <c r="P32" s="100"/>
       <c r="Q32" s="117"/>
       <c r="R32" s="28"/>
       <c r="S32" s="28"/>
@@ -3792,7 +3792,7 @@
       <c r="L33" s="45"/>
       <c r="M33" s="38">
         <f>IF(ISBLANK(L33), NETWORKDAYS(J34, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J34, L33, Hoja2!$A$1:$A$18))</f>
-        <v>32768</v>
+        <v>32770</v>
       </c>
       <c r="N33" s="46"/>
       <c r="O33" s="47"/>
@@ -3836,11 +3836,11 @@
       <c r="L34" s="87"/>
       <c r="M34" s="23">
         <f>IF(ISBLANK(L34), NETWORKDAYS(J35, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J35, L34, Hoja2!$A$1:$A$18))</f>
-        <v>32768</v>
+        <v>32770</v>
       </c>
       <c r="N34" s="90"/>
       <c r="O34" s="50"/>
-      <c r="P34" s="99"/>
+      <c r="P34" s="100"/>
       <c r="Q34" s="117"/>
       <c r="R34" s="28"/>
       <c r="S34" s="28"/>
@@ -3880,7 +3880,7 @@
       <c r="L35" s="45"/>
       <c r="M35" s="38">
         <f>IF(ISBLANK(L35), NETWORKDAYS(J36, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J36, L35, Hoja2!$A$1:$A$18))</f>
-        <v>32768</v>
+        <v>32770</v>
       </c>
       <c r="N35" s="46"/>
       <c r="O35" s="47"/>
@@ -3924,11 +3924,11 @@
       <c r="L36" s="87"/>
       <c r="M36" s="23">
         <f>IF(ISBLANK(L36), NETWORKDAYS(J37, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J37, L36, Hoja2!$A$1:$A$18))</f>
-        <v>32768</v>
+        <v>32770</v>
       </c>
       <c r="N36" s="90"/>
       <c r="O36" s="50"/>
-      <c r="P36" s="99"/>
+      <c r="P36" s="100"/>
       <c r="Q36" s="117"/>
       <c r="R36" s="28"/>
       <c r="S36" s="28"/>
@@ -3968,7 +3968,7 @@
       <c r="L37" s="45"/>
       <c r="M37" s="38">
         <f>IF(ISBLANK(L37), NETWORKDAYS(J38, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J38, L37, Hoja2!$A$1:$A$18))</f>
-        <v>32768</v>
+        <v>32770</v>
       </c>
       <c r="N37" s="46"/>
       <c r="O37" s="47"/>
@@ -4012,11 +4012,11 @@
       <c r="L38" s="87"/>
       <c r="M38" s="23">
         <f>IF(ISBLANK(L38), NETWORKDAYS(J39, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J39, L38, Hoja2!$A$1:$A$18))</f>
-        <v>32768</v>
+        <v>32770</v>
       </c>
       <c r="N38" s="90"/>
       <c r="O38" s="50"/>
-      <c r="P38" s="99"/>
+      <c r="P38" s="100"/>
       <c r="Q38" s="117"/>
       <c r="R38" s="28"/>
       <c r="S38" s="28"/>

</xml_diff>